<commit_message>
Lab & General Billing Reviewed
</commit_message>
<xml_diff>
--- a/Test Cases/Nithya/Test Case- Lab & General Billing - Reviewed.xlsx
+++ b/Test Cases/Nithya/Test Case- Lab & General Billing - Reviewed.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1678" uniqueCount="519">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1747" uniqueCount="553">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -2399,6 +2399,139 @@
       </rPr>
       <t xml:space="preserve"> advance entry should be made</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Precondition:The Patient should be consulted and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>advance entry should be made</t>
+    </r>
+  </si>
+  <si>
+    <t>Search patient page should be opened.
+A table with patient details should be displayed</t>
+  </si>
+  <si>
+    <t>MED_LGB_TC_074</t>
+  </si>
+  <si>
+    <t>Verify Summary Information table under Billing Search</t>
+  </si>
+  <si>
+    <t>Navigate to Billing search tab</t>
+  </si>
+  <si>
+    <t>Billing serach page should be displayed</t>
+  </si>
+  <si>
+    <t>Summary Information table should contian:
+-Today's Bills
+-Op Bills
+-IP Bills
+-Credit Bills
+-Cash Bills
+-Complimentary Bills
+-Pending Request
+-Emergency Bills</t>
+  </si>
+  <si>
+    <t>MED_LGB_TC_075</t>
+  </si>
+  <si>
+    <t>Verify on clicking Billed status, user gets navigated to lab and general billing page</t>
+  </si>
+  <si>
+    <t>Precondition:The Patient should be consulted and Billed</t>
+  </si>
+  <si>
+    <t>#NH00000596 - Arjun</t>
+  </si>
+  <si>
+    <t>Verify page gets navigated to lab and General Billing page</t>
+  </si>
+  <si>
+    <t>lab and General Billing page should be displayed</t>
+  </si>
+  <si>
+    <t>patient should get listed</t>
+  </si>
+  <si>
+    <t>MED_LGB_TC_076</t>
+  </si>
+  <si>
+    <t>Verify Editing Todays Bills</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Search for a Billed  patient on entering data in fields upon clciking show option </t>
+  </si>
+  <si>
+    <t>Once patient is displayed under Todays Bills, click on Billed status</t>
+  </si>
+  <si>
+    <t>Once patient is displayed under Todays Bills, click on Edit option</t>
+  </si>
+  <si>
+    <t>Make changes and save it for verification</t>
+  </si>
+  <si>
+    <t>Edited fields should be saved</t>
+  </si>
+  <si>
+    <t>Precondition:The Patient should be consulted and Billed
+Navigate to Application Selector&gt;&gt;Select Lab and General Billing</t>
+  </si>
+  <si>
+    <t>MED_LGB_TC_077</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Precondition:The Patient should be consulted and Billed
+</t>
+  </si>
+  <si>
+    <t>Click on Linked patients option and verify result</t>
+  </si>
+  <si>
+    <t>Verify Linked patients</t>
+  </si>
+  <si>
+    <t>Linked patients should be displayed</t>
+  </si>
+  <si>
+    <t>MED_LGB_TC_078</t>
+  </si>
+  <si>
+    <t>Verify data displayed in Summary Information table on selecting different dates from date picker</t>
+  </si>
+  <si>
+    <t>Navigate to dashboard tab</t>
+  </si>
+  <si>
+    <t>Dashboard page should be displayed</t>
+  </si>
+  <si>
+    <t>Summary Information table should contain:
+-Today's Bills
+-Op Bills
+-IP Bills
+-Credit Bills
+-Cash Bills
+-Complimentary Bills
+-Pending Request
+-Emergency Bills</t>
+  </si>
+  <si>
+    <t>Verify Summary Information table under dashboard of Todays Bill summary</t>
+  </si>
+  <si>
+    <t>http://mediwarecloud.com</t>
   </si>
 </sst>
 </file>
@@ -2487,7 +2620,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2509,6 +2642,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2550,7 +2695,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2630,15 +2775,25 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2954,11 +3109,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S734"/>
+  <dimension ref="A1:S744"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A432" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F433" sqref="F433"/>
+      <pane ySplit="1" topLeftCell="A739" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H722" sqref="H722"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3015,14 +3170,14 @@
       <c r="M1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="27" t="s">
+      <c r="O1" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="27"/>
-      <c r="R1" s="28" t="s">
+      <c r="P1" s="31"/>
+      <c r="R1" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="S1" s="28"/>
+      <c r="S1" s="32"/>
     </row>
     <row r="2" spans="1:19" s="9" customFormat="1" ht="33.75" customHeight="1">
       <c r="A2" s="15" t="s">
@@ -3057,7 +3212,7 @@
       </c>
       <c r="P2" s="11">
         <f>COUNTA(A:A)-1</f>
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="R2" s="12" t="s">
         <v>12</v>
@@ -3642,7 +3797,7 @@
       <c r="L41" s="8"/>
     </row>
     <row r="42" spans="1:12" ht="45">
-      <c r="A42" s="29" t="s">
+      <c r="A42" s="27" t="s">
         <v>22</v>
       </c>
       <c r="B42" s="18" t="s">
@@ -4334,7 +4489,7 @@
       <c r="L91" s="8"/>
     </row>
     <row r="92" spans="1:12" ht="45">
-      <c r="A92" s="6" t="s">
+      <c r="A92" s="28" t="s">
         <v>26</v>
       </c>
       <c r="B92" s="18" t="s">
@@ -4507,7 +4662,7 @@
       <c r="L104" s="8"/>
     </row>
     <row r="105" spans="1:12" ht="60">
-      <c r="A105" s="6" t="s">
+      <c r="A105" s="28" t="s">
         <v>27</v>
       </c>
       <c r="B105" s="18" t="s">
@@ -4705,7 +4860,7 @@
       <c r="L118" s="8"/>
     </row>
     <row r="119" spans="1:12" ht="60">
-      <c r="A119" s="6" t="s">
+      <c r="A119" s="28" t="s">
         <v>28</v>
       </c>
       <c r="B119" s="18" t="s">
@@ -4848,7 +5003,7 @@
         <v>10</v>
       </c>
       <c r="F128" s="6" t="s">
-        <v>105</v>
+        <v>59</v>
       </c>
       <c r="G128" s="6" t="s">
         <v>114</v>
@@ -4903,7 +5058,7 @@
       <c r="L132" s="8"/>
     </row>
     <row r="133" spans="1:12" ht="45">
-      <c r="A133" s="6" t="s">
+      <c r="A133" s="28" t="s">
         <v>29</v>
       </c>
       <c r="B133" s="18" t="s">
@@ -5046,7 +5201,7 @@
         <v>10</v>
       </c>
       <c r="F142" s="6" t="s">
-        <v>105</v>
+        <v>59</v>
       </c>
       <c r="G142" s="6" t="s">
         <v>114</v>
@@ -5085,7 +5240,7 @@
       <c r="L145" s="8"/>
     </row>
     <row r="146" spans="1:12" ht="45">
-      <c r="A146" s="6" t="s">
+      <c r="A146" s="28" t="s">
         <v>30</v>
       </c>
       <c r="B146" s="18" t="s">
@@ -5228,7 +5383,7 @@
         <v>10</v>
       </c>
       <c r="F155" s="6" t="s">
-        <v>105</v>
+        <v>59</v>
       </c>
       <c r="G155" s="6" t="s">
         <v>114</v>
@@ -5280,7 +5435,7 @@
       <c r="L159" s="8"/>
     </row>
     <row r="160" spans="1:12" ht="75">
-      <c r="A160" s="6" t="s">
+      <c r="A160" s="28" t="s">
         <v>31</v>
       </c>
       <c r="B160" s="18" t="s">
@@ -5491,7 +5646,7 @@
       <c r="L174" s="8"/>
     </row>
     <row r="175" spans="1:12" ht="60">
-      <c r="A175" s="6" t="s">
+      <c r="A175" s="28" t="s">
         <v>32</v>
       </c>
       <c r="B175" s="18" t="s">
@@ -5686,7 +5841,7 @@
       <c r="L188" s="8"/>
     </row>
     <row r="189" spans="1:12" ht="75">
-      <c r="A189" s="6" t="s">
+      <c r="A189" s="28" t="s">
         <v>33</v>
       </c>
       <c r="B189" s="18" t="s">
@@ -5880,13 +6035,13 @@
       <c r="L201" s="8"/>
     </row>
     <row r="202" spans="1:12">
-      <c r="A202" s="6" t="s">
-        <v>34</v>
-      </c>
       <c r="K202" s="4"/>
       <c r="L202" s="8"/>
     </row>
     <row r="203" spans="1:12" ht="90">
+      <c r="A203" s="28" t="s">
+        <v>34</v>
+      </c>
       <c r="B203" s="18" t="s">
         <v>36</v>
       </c>
@@ -6027,7 +6182,7 @@
         <v>10</v>
       </c>
       <c r="F212" s="6" t="s">
-        <v>105</v>
+        <v>59</v>
       </c>
       <c r="G212" s="6" t="s">
         <v>114</v>
@@ -6098,7 +6253,7 @@
       <c r="L217" s="8"/>
     </row>
     <row r="218" spans="1:12" ht="45">
-      <c r="A218" s="6" t="s">
+      <c r="A218" s="28" t="s">
         <v>139</v>
       </c>
       <c r="B218" s="18" t="s">
@@ -6241,7 +6396,7 @@
         <v>10</v>
       </c>
       <c r="F227" s="6" t="s">
-        <v>105</v>
+        <v>59</v>
       </c>
       <c r="G227" s="6" t="s">
         <v>114</v>
@@ -6280,7 +6435,7 @@
       <c r="L230" s="8"/>
     </row>
     <row r="231" spans="1:12" ht="45">
-      <c r="A231" s="6" t="s">
+      <c r="A231" s="28" t="s">
         <v>144</v>
       </c>
       <c r="B231" s="18" t="s">
@@ -6465,7 +6620,7 @@
       <c r="L243" s="8"/>
     </row>
     <row r="244" spans="1:12" ht="45">
-      <c r="A244" s="6" t="s">
+      <c r="A244" s="28" t="s">
         <v>147</v>
       </c>
       <c r="B244" s="18" t="s">
@@ -6647,7 +6802,7 @@
       <c r="L256" s="8"/>
     </row>
     <row r="257" spans="1:12" ht="45">
-      <c r="A257" s="6" t="s">
+      <c r="A257" s="28" t="s">
         <v>149</v>
       </c>
       <c r="B257" s="18" t="s">
@@ -6832,7 +6987,7 @@
       <c r="L269" s="8"/>
     </row>
     <row r="270" spans="1:12" ht="45">
-      <c r="A270" s="6" t="s">
+      <c r="A270" s="28" t="s">
         <v>168</v>
       </c>
       <c r="B270" s="18" t="s">
@@ -7030,7 +7185,7 @@
       <c r="L283" s="8"/>
     </row>
     <row r="284" spans="1:12" ht="45">
-      <c r="A284" s="6" t="s">
+      <c r="A284" s="28" t="s">
         <v>184</v>
       </c>
       <c r="B284" s="18" t="s">
@@ -7170,7 +7325,7 @@
         <v>10</v>
       </c>
       <c r="F293" s="6" t="s">
-        <v>105</v>
+        <v>59</v>
       </c>
       <c r="G293" s="6" t="s">
         <v>114</v>
@@ -7951,7 +8106,7 @@
       <c r="J348" s="4"/>
       <c r="K348" s="8"/>
     </row>
-    <row r="349" spans="1:18" s="9" customFormat="1" ht="25.5" customHeight="1">
+    <row r="349" spans="1:18" s="9" customFormat="1" ht="241.5" customHeight="1">
       <c r="A349" s="6"/>
       <c r="B349" s="21"/>
       <c r="C349" s="4"/>
@@ -8950,7 +9105,7 @@
         <v>257</v>
       </c>
       <c r="F420" s="6" t="s">
-        <v>146</v>
+        <v>519</v>
       </c>
       <c r="I420" s="6" t="s">
         <v>62</v>
@@ -9974,7 +10129,7 @@
       <c r="L494" s="8"/>
     </row>
     <row r="495" spans="1:12" ht="45">
-      <c r="A495" s="6" t="s">
+      <c r="A495" s="29" t="s">
         <v>300</v>
       </c>
       <c r="B495" s="18" t="s">
@@ -10056,7 +10211,7 @@
         <v>304</v>
       </c>
       <c r="G500" s="23" t="s">
-        <v>305</v>
+        <v>520</v>
       </c>
       <c r="K500" s="8"/>
       <c r="L500" s="8"/>
@@ -10065,7 +10220,7 @@
       <c r="E501" s="22">
         <v>6</v>
       </c>
-      <c r="F501" s="22" t="s">
+      <c r="F501" s="30" t="s">
         <v>306</v>
       </c>
       <c r="G501" s="23" t="s">
@@ -12857,63 +13012,351 @@
     <row r="715" spans="1:12">
       <c r="L715" s="8"/>
     </row>
-    <row r="716" spans="1:12">
-      <c r="B716" s="18"/>
+    <row r="716" spans="1:12" ht="45">
+      <c r="A716" s="6" t="s">
+        <v>521</v>
+      </c>
+      <c r="B716" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D716" s="6" t="s">
+        <v>522</v>
+      </c>
+      <c r="F716" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="H716" s="33"/>
+      <c r="I716" s="33" t="s">
+        <v>552</v>
+      </c>
       <c r="L716" s="8"/>
     </row>
-    <row r="717" spans="1:12">
+    <row r="717" spans="1:12" ht="65.25" customHeight="1">
+      <c r="E717" s="6">
+        <v>1</v>
+      </c>
+      <c r="F717" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G717" s="6" t="s">
+        <v>43</v>
+      </c>
       <c r="L717" s="8"/>
     </row>
-    <row r="718" spans="1:12">
+    <row r="718" spans="1:12" ht="30">
+      <c r="E718" s="6">
+        <v>2</v>
+      </c>
+      <c r="F718" s="6" t="s">
+        <v>523</v>
+      </c>
+      <c r="G718" s="6" t="s">
+        <v>524</v>
+      </c>
       <c r="L718" s="8"/>
     </row>
-    <row r="719" spans="1:12">
+    <row r="719" spans="1:12" ht="150">
+      <c r="E719" s="6">
+        <v>3</v>
+      </c>
+      <c r="F719" s="6" t="s">
+        <v>547</v>
+      </c>
+      <c r="G719" s="6" t="s">
+        <v>525</v>
+      </c>
       <c r="L719" s="8"/>
     </row>
     <row r="720" spans="1:12">
       <c r="L720" s="8"/>
     </row>
-    <row r="721" spans="12:12">
+    <row r="721" spans="1:12" ht="60">
+      <c r="A721" s="6" t="s">
+        <v>526</v>
+      </c>
+      <c r="B721" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D721" s="6" t="s">
+        <v>527</v>
+      </c>
+      <c r="F721" s="6" t="s">
+        <v>528</v>
+      </c>
+      <c r="H721" s="33"/>
+      <c r="I721" s="33" t="s">
+        <v>552</v>
+      </c>
       <c r="L721" s="8"/>
     </row>
-    <row r="722" spans="12:12">
+    <row r="722" spans="1:12" ht="33" customHeight="1">
+      <c r="E722" s="6">
+        <v>1</v>
+      </c>
+      <c r="F722" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G722" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="I722" s="6" t="s">
+        <v>529</v>
+      </c>
       <c r="L722" s="8"/>
     </row>
-    <row r="723" spans="12:12">
+    <row r="723" spans="1:12" ht="35.25" customHeight="1">
+      <c r="E723" s="6">
+        <v>2</v>
+      </c>
+      <c r="F723" s="6" t="s">
+        <v>523</v>
+      </c>
+      <c r="G723" s="6" t="s">
+        <v>524</v>
+      </c>
       <c r="L723" s="8"/>
     </row>
-    <row r="724" spans="12:12">
+    <row r="724" spans="1:12" ht="30">
+      <c r="E724" s="6">
+        <v>3</v>
+      </c>
+      <c r="F724" s="6" t="s">
+        <v>535</v>
+      </c>
+      <c r="G724" s="6" t="s">
+        <v>532</v>
+      </c>
       <c r="L724" s="8"/>
     </row>
-    <row r="725" spans="12:12">
+    <row r="725" spans="1:12" ht="30">
+      <c r="E725" s="6">
+        <v>4</v>
+      </c>
+      <c r="F725" s="6" t="s">
+        <v>536</v>
+      </c>
+      <c r="G725" s="6" t="s">
+        <v>531</v>
+      </c>
       <c r="L725" s="8"/>
     </row>
-    <row r="726" spans="12:12">
+    <row r="726" spans="1:12" ht="30">
+      <c r="E726" s="6">
+        <v>5</v>
+      </c>
+      <c r="F726" s="6" t="s">
+        <v>530</v>
+      </c>
+      <c r="G726" s="6" t="s">
+        <v>531</v>
+      </c>
       <c r="L726" s="8"/>
     </row>
-    <row r="727" spans="12:12">
+    <row r="727" spans="1:12">
       <c r="L727" s="8"/>
     </row>
-    <row r="728" spans="12:12">
+    <row r="728" spans="1:12" ht="79.5" customHeight="1">
+      <c r="A728" s="6" t="s">
+        <v>533</v>
+      </c>
+      <c r="B728" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D728" s="6" t="s">
+        <v>534</v>
+      </c>
+      <c r="E728" s="6">
+        <v>1</v>
+      </c>
+      <c r="F728" s="6" t="s">
+        <v>540</v>
+      </c>
+      <c r="G728" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="I728" s="33" t="s">
+        <v>552</v>
+      </c>
       <c r="L728" s="8"/>
     </row>
-    <row r="729" spans="12:12">
+    <row r="729" spans="1:12" ht="30">
+      <c r="E729" s="6">
+        <v>2</v>
+      </c>
+      <c r="F729" s="6" t="s">
+        <v>523</v>
+      </c>
+      <c r="G729" s="6" t="s">
+        <v>524</v>
+      </c>
+      <c r="I729" s="6" t="s">
+        <v>529</v>
+      </c>
       <c r="L729" s="8"/>
     </row>
-    <row r="730" spans="12:12">
+    <row r="730" spans="1:12" ht="30">
+      <c r="E730" s="6">
+        <v>3</v>
+      </c>
+      <c r="F730" s="6" t="s">
+        <v>535</v>
+      </c>
+      <c r="G730" s="6" t="s">
+        <v>532</v>
+      </c>
       <c r="L730" s="8"/>
     </row>
-    <row r="731" spans="12:12">
+    <row r="731" spans="1:12" ht="30">
+      <c r="E731" s="6">
+        <v>4</v>
+      </c>
+      <c r="F731" s="6" t="s">
+        <v>537</v>
+      </c>
+      <c r="G731" s="6" t="s">
+        <v>43</v>
+      </c>
       <c r="L731" s="8"/>
     </row>
-    <row r="732" spans="12:12">
+    <row r="732" spans="1:12">
+      <c r="E732" s="6">
+        <v>5</v>
+      </c>
+      <c r="F732" s="6" t="s">
+        <v>538</v>
+      </c>
+      <c r="G732" s="6" t="s">
+        <v>539</v>
+      </c>
       <c r="L732" s="8"/>
     </row>
-    <row r="733" spans="12:12">
+    <row r="733" spans="1:12">
       <c r="L733" s="8"/>
     </row>
-    <row r="734" spans="12:12">
-      <c r="L734" s="8"/>
+    <row r="734" spans="1:12" ht="45">
+      <c r="A734" s="6" t="s">
+        <v>541</v>
+      </c>
+      <c r="B734" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D734" s="6" t="s">
+        <v>544</v>
+      </c>
+      <c r="F734" s="6" t="s">
+        <v>542</v>
+      </c>
+      <c r="I734" s="33" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="735" spans="1:12" ht="30">
+      <c r="E735" s="6">
+        <v>1</v>
+      </c>
+      <c r="F735" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G735" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="736" spans="1:12" ht="30">
+      <c r="E736" s="6">
+        <v>2</v>
+      </c>
+      <c r="F736" s="6" t="s">
+        <v>523</v>
+      </c>
+      <c r="G736" s="6" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="737" spans="1:9" ht="30">
+      <c r="E737" s="6">
+        <v>3</v>
+      </c>
+      <c r="F737" s="6" t="s">
+        <v>535</v>
+      </c>
+      <c r="G737" s="6" t="s">
+        <v>532</v>
+      </c>
+      <c r="I737" s="6" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="738" spans="1:9" ht="30">
+      <c r="E738" s="6">
+        <v>4</v>
+      </c>
+      <c r="F738" s="6" t="s">
+        <v>537</v>
+      </c>
+      <c r="G738" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="739" spans="1:9" ht="30">
+      <c r="E739" s="6">
+        <v>5</v>
+      </c>
+      <c r="F739" s="6" t="s">
+        <v>543</v>
+      </c>
+      <c r="G739" s="6" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="741" spans="1:9" ht="60">
+      <c r="A741" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="B741" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D741" s="6" t="s">
+        <v>551</v>
+      </c>
+      <c r="F741" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="I741" s="33" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="742" spans="1:9" ht="30">
+      <c r="E742" s="6">
+        <v>1</v>
+      </c>
+      <c r="F742" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G742" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="743" spans="1:9" ht="30">
+      <c r="E743" s="6">
+        <v>2</v>
+      </c>
+      <c r="F743" s="6" t="s">
+        <v>548</v>
+      </c>
+      <c r="G743" s="6" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="744" spans="1:9" ht="150">
+      <c r="E744" s="6">
+        <v>3</v>
+      </c>
+      <c r="F744" s="6" t="s">
+        <v>547</v>
+      </c>
+      <c r="G744" s="6" t="s">
+        <v>550</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -12924,13 +13367,13 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K346 J347:J356 K357:K485 C2:C662 C672 C716">
       <formula1>"Nithya VS, Poonima John, Prapancha, Preethi Pathrose, Semin Das, Sangeetha, Rijo J Patric"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C663:C671 C673:C715 C717:C730">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C663:C671 C673:C715 C717:C729">
       <formula1>"Nithya VS, Poonima John, Prapancha, Preethi Pathrose, Parvathy P, Semin Das, Sangeetha, Rijo J Patric"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 B56 B13 B23 B30 B42 B69 B79 B92 B105 B119 B133 B146 B160 B175 B189 B203 B218 B231 B244 B257 B270 B284 B298 B309 B320 B333 B345 B347:B356 B361 B371 B381 B390 B400 B411 B420 B429 B437 B445 B453 B460 B467 B474 B481 B488 B495 B503 B509 B517 B525 B532 B539 B545 B551 B557 B563 B569 B576 B583 B592 B599 B608 B617 B626 B635 B644 B653 B660 B672 B681 B691 B698 B707 B716">
       <formula1>"CAS/ Appointment, Out Patient, Care Desk, EMR, Lab &amp; General Billing, Pharmacy Billing, Lab Results, Radiology, Insurance Desk, Casualty, MRD, In Patient, Nursing Station, Theatre, Indent, Store Management"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L346 K347:K356 L357:L734">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L346 K347:K356 L357:L733">
       <formula1>"Pass, Fail, Blocked"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K486:K689">
@@ -12939,8 +13382,13 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1"/>
+    <hyperlink ref="I716" r:id="rId2" display="http://mediwarecloud.com/"/>
+    <hyperlink ref="I721" r:id="rId3" display="http://mediwarecloud.com/"/>
+    <hyperlink ref="I728" r:id="rId4" display="http://mediwarecloud.com/"/>
+    <hyperlink ref="I734" r:id="rId5" display="http://mediwarecloud.com/"/>
+    <hyperlink ref="I741" r:id="rId6" display="http://mediwarecloud.com/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>